<commit_message>
added all reports & fixed some issues
</commit_message>
<xml_diff>
--- a/testdata/test_data.xlsx
+++ b/testdata/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2421185\Documents\JustDail\IdentifyCarWashes\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFB8C47-F939-410F-AA78-8A379CF70EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194D1FB6-CE34-4522-9F38-B79C3FC397F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{039457C7-6789-4A31-AFFF-AE509E2716E5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Location</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Kandivali, Mumbai</t>
-  </si>
-  <si>
-    <t>Mira Road East, Thane</t>
   </si>
   <si>
     <t>Vasai East, Palghar</t>
@@ -157,9 +154,6 @@
   </si>
   <si>
     <t>Car Washing Services</t>
-  </si>
-  <si>
-    <t>Gyms</t>
   </si>
   <si>
     <t>Education Consultants</t>
@@ -579,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E215CD4-C1F2-4F00-BF07-B894E942C1B4}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -622,16 +616,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -642,7 +636,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>18</v>
@@ -651,18 +645,18 @@
         <v>22</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>19</v>
@@ -671,7 +665,7 @@
         <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -679,19 +673,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -702,16 +696,16 @@
         <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -719,19 +713,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -739,16 +733,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>25</v>
@@ -765,33 +759,13 @@
         <v>15</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed handling location problem
</commit_message>
<xml_diff>
--- a/testdata/test_data.xlsx
+++ b/testdata/test_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2421185\Documents\JustDail\IdentifyCarWashes\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dinesh\java\Hackathon\IdentifyServices\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194D1FB6-CE34-4522-9F38-B79C3FC397F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B07BF7F-0FAC-447B-9F89-C3AE3883E7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{039457C7-6789-4A31-AFFF-AE509E2716E5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Location</t>
   </si>
@@ -62,43 +62,6 @@
     <t>Vasai East, Palghar</t>
   </si>
   <si>
-    <t>Calcutta Boys School Entally, Kolkata</t>
-  </si>
-  <si>
-    <t>Muvattupuzha, Ernakulam</t>
-  </si>
-  <si>
-    <t>Kondapur, Hyderabad</t>
-  </si>
-  <si>
-    <r>
-      <t>Ahmedabad</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> Palace Road, Bhopal</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Vishaka</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>patnam Central Suryabagh, Visakhapatnam</t>
-    </r>
-  </si>
-  <si>
     <t>Pet Shops</t>
   </si>
   <si>
@@ -160,6 +123,18 @@
   </si>
   <si>
     <t>Paying Guest</t>
+  </si>
+  <si>
+    <t>Mira Road East, Thane</t>
+  </si>
+  <si>
+    <t>Malad West, Mumbai</t>
+  </si>
+  <si>
+    <t>Thane West, Thane</t>
+  </si>
+  <si>
+    <t>Mumbai Central, Mumbai</t>
   </si>
 </sst>
 </file>
@@ -576,7 +551,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -616,16 +591,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -636,16 +611,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -653,19 +628,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -673,19 +648,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -693,19 +668,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -713,19 +688,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -733,19 +708,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -753,19 +728,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>